<commit_message>
adding the new code
</commit_message>
<xml_diff>
--- a/Results/Results/result analysis_Latest.xlsx
+++ b/Results/Results/result analysis_Latest.xlsx
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2794,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,12 +3413,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>